<commit_message>
location filter code update
</commit_message>
<xml_diff>
--- a/data/hme/transformed/hme_transformed.xlsx
+++ b/data/hme/transformed/hme_transformed.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Dunkin-sales-summary\data\hme\transformed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A0C54B-1660-4BBD-B72F-0C1FEC02E622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-23220" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -97,11 +103,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -149,29 +155,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -209,7 +235,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -243,6 +269,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -277,9 +304,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,14 +480,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T10" sqref="Q1:T10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +538,11 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45906</v>
       </c>
@@ -553,7 +589,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45906</v>
       </c>
@@ -600,7 +636,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45906</v>
       </c>
@@ -647,7 +683,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45906</v>
       </c>
@@ -694,7 +730,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45906</v>
       </c>
@@ -741,7 +777,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45906</v>
       </c>
@@ -788,7 +824,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45906</v>
       </c>
@@ -835,7 +871,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45906</v>
       </c>
@@ -882,7 +918,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45906</v>
       </c>
@@ -929,7 +965,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45906</v>
       </c>
@@ -976,7 +1012,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45906</v>
       </c>
@@ -1023,7 +1059,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45906</v>
       </c>
@@ -1070,7 +1106,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45906</v>
       </c>
@@ -1117,7 +1153,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45906</v>
       </c>
@@ -1164,7 +1200,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45906</v>
       </c>
@@ -1211,7 +1247,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45906</v>
       </c>
@@ -1258,7 +1294,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45906</v>
       </c>
@@ -1305,7 +1341,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45906</v>
       </c>
@@ -1352,7 +1388,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45906</v>
       </c>
@@ -1399,7 +1435,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45906</v>
       </c>
@@ -1446,7 +1482,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45906</v>
       </c>
@@ -1493,7 +1529,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45906</v>
       </c>
@@ -1540,7 +1576,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45906</v>
       </c>
@@ -1587,7 +1623,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45906</v>
       </c>
@@ -1634,7 +1670,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45906</v>
       </c>
@@ -1683,5 +1719,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>